<commit_message>
Cambios en entidades, nueva entidad mensajes, corrección documentación
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5439EE-67D2-4643-8CAA-B028A1ACE1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C004DFFD-A526-4A4C-910C-8889E9431C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -318,12 +318,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,23 +358,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>23417</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>44717</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>597018</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ED3FA79-E8EE-ED8B-9E78-56C7D651CA17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF0A75B-23F8-1AA5-9F35-3E46D9934A67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -398,8 +396,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4686300" y="5514975"/>
-          <a:ext cx="6367067" cy="3321317"/>
+          <a:off x="16678275" y="190500"/>
+          <a:ext cx="6073893" cy="7372350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,7 +675,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +703,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="8"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
@@ -720,22 +718,22 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="1" t="s">
         <v>39</v>
       </c>
@@ -743,22 +741,22 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5"/>
       <c r="J3" s="1" t="s">
         <v>40</v>
       </c>
@@ -766,22 +764,22 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5"/>
       <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
@@ -789,22 +787,22 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5"/>
       <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
@@ -812,22 +810,22 @@
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
         <v>43</v>
       </c>
@@ -835,378 +833,378 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5"/>
       <c r="J7" s="1"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="1"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="5"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="5"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5"/>
       <c r="J12" s="1"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="1"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="5"/>
+      <c r="F14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="1"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="11" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="5"/>
       <c r="J15" s="1"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="1"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="11" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="5"/>
       <c r="J18" s="1"/>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="10" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="5"/>
       <c r="J19" s="1"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="5"/>
       <c r="J20" s="1"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="12" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="5"/>
       <c r="J21" s="1"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="5"/>
+      <c r="F22" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="5"/>
       <c r="J22" s="1"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="13" t="s">
+      <c r="E23" s="5"/>
+      <c r="F23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="6"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="5"/>
       <c r="J23" s="1"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="13" t="s">
+      <c r="E24" s="5"/>
+      <c r="F24" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="5"/>
       <c r="J24" s="1"/>
       <c r="K24" s="3"/>
     </row>
@@ -1216,8 +1214,8 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>

</xml_diff>

<commit_message>
Seguridad y método crear cliente usuario
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C004DFFD-A526-4A4C-910C-8889E9431C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4197888-C4AA-4C04-B80B-BC08E3F6EC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Eliminar el cliente pero no sus citas, se dejarán con el cliente a null y se mostrará su nombre y apellidos</t>
+  </si>
+  <si>
+    <t>Como OCASIONAL, quiero loguearme</t>
+  </si>
+  <si>
+    <t>Formulario de login</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -304,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -336,6 +345,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +702,7 @@
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
     <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
@@ -753,8 +768,8 @@
         <v>53</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="7" t="s">
-        <v>4</v>
+      <c r="H3" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="1" t="s">
@@ -763,17 +778,17 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
+      <c r="D4" t="s">
+        <v>63</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="9" t="s">
-        <v>54</v>
+      <c r="F4" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="7" t="s">
@@ -788,15 +803,15 @@
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -811,15 +826,15 @@
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="8" t="s">
-        <v>53</v>
+      <c r="F6" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
@@ -834,15 +849,15 @@
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="10" t="s">
-        <v>57</v>
+      <c r="F7" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="7" t="s">
@@ -855,15 +870,15 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="11" t="s">
-        <v>58</v>
+      <c r="F8" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
@@ -876,15 +891,15 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="8" t="s">
-        <v>59</v>
+      <c r="F9" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="7" t="s">
@@ -897,15 +912,15 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="10" t="s">
-        <v>57</v>
+      <c r="F10" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="7" t="s">
@@ -916,17 +931,17 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="11" t="s">
-        <v>58</v>
+      <c r="F11" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="7" t="s">
@@ -936,17 +951,17 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="9" t="s">
-        <v>55</v>
+      <c r="F12" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="7" t="s">
@@ -959,7 +974,7 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
@@ -980,11 +995,11 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="9" t="s">
@@ -1001,15 +1016,15 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="7" t="s">
@@ -1022,11 +1037,11 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9" t="s">
@@ -1043,11 +1058,11 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9" t="s">
@@ -1064,15 +1079,15 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="8" t="s">
-        <v>53</v>
+      <c r="F18" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="7" t="s">
@@ -1085,11 +1100,11 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="8" t="s">
@@ -1106,15 +1121,15 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="10" t="s">
-        <v>57</v>
+      <c r="F20" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="7" t="s">
@@ -1124,14 +1139,14 @@
       <c r="J20" s="1"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="10" t="s">
@@ -1145,18 +1160,18 @@
       <c r="J21" s="1"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="8" t="s">
-        <v>59</v>
+      <c r="F22" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7" t="s">
@@ -1166,18 +1181,18 @@
       <c r="J22" s="1"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="11" t="s">
-        <v>58</v>
+      <c r="F23" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="7" t="s">
@@ -1187,14 +1202,14 @@
       <c r="J23" s="1"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="11" t="s">
@@ -1210,16 +1225,37 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="5"/>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="G25" s="5"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="H25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios en seguridad, y petición login
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543D0DCD-C4B8-48DB-95CE-0AF24C37EB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666A954D-5C48-4727-819D-94A98A6848BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Como ADMIN-MEC, quiero ver los detalles de un cliente</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC, quiero ver los detalles de un mecánico</t>
-  </si>
-  <si>
     <t>Como ADMIN-MEC, quiero ver los detalles de una cita</t>
   </si>
   <si>
@@ -210,19 +207,34 @@
     <t>Como HABITUAL, quiero darme de baja</t>
   </si>
   <si>
-    <t>Eliminar el cliente pero no sus citas, se dejarán con el cliente a null y se mostrará su nombre y apellidos</t>
-  </si>
-  <si>
     <t>Como OCASIONAL, quiero loguearme</t>
   </si>
   <si>
     <t>Formulario de login</t>
   </si>
   <si>
-    <t>PROGRESS</t>
-  </si>
-  <si>
-    <t>PROGRESS FALTA SWAGGER Y MOSTRAR DATOS EN BONITO</t>
+    <t>FLUTTER</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero crear un admin</t>
+  </si>
+  <si>
+    <t>Crear un nuevo admin</t>
+  </si>
+  <si>
+    <t>Eliminar el cliente pero no sus citas, se dejarán con el cliente a null y se mostrará su nombre y apellidos. Solo podrá borrarse a sí mismo</t>
+  </si>
+  <si>
+    <t>Como HABITUAL, quiero modificar mi contraseña</t>
+  </si>
+  <si>
+    <t>Obligatorio poner la antigua para comprobar que está bien, y dos veces la nueva que no coincida con antigua</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC, quiero ver los detalles personales</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC, quiero cambiar mi contraseña</t>
   </si>
 </sst>
 </file>
@@ -254,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +315,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -316,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,10 +367,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,7 +403,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>597018</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -688,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +741,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="2" t="s">
@@ -734,31 +755,31 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="1" t="s">
@@ -766,38 +787,38 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="12" t="s">
-        <v>64</v>
+      <c r="H3" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="7" t="s">
-        <v>4</v>
+      <c r="H4" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -812,7 +833,7 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
@@ -820,7 +841,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -831,11 +852,11 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
@@ -843,7 +864,7 @@
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -854,11 +875,11 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="7" t="s">
@@ -875,11 +896,11 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
@@ -896,11 +917,11 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="7" t="s">
@@ -917,11 +938,11 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="7" t="s">
@@ -942,7 +963,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="7" t="s">
@@ -951,39 +972,38 @@
       <c r="I11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="11" t="s">
-        <v>58</v>
+      <c r="F12" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="9" t="s">
-        <v>55</v>
+      <c r="F13" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="7" t="s">
@@ -996,15 +1016,15 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="7" t="s">
@@ -1017,15 +1037,15 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="7" t="s">
@@ -1038,11 +1058,11 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9" t="s">
@@ -1059,15 +1079,15 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="7" t="s">
@@ -1080,7 +1100,7 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
@@ -1088,7 +1108,7 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="7" t="s">
@@ -1101,14 +1121,14 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G19" s="5"/>
@@ -1120,38 +1140,37 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="5"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="3"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="10" t="s">
-        <v>57</v>
+      <c r="F21" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="7" t="s">
@@ -1162,38 +1181,37 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="3"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="8" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="7" t="s">
@@ -1203,18 +1221,18 @@
       <c r="J23" s="1"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="11" t="s">
-        <v>58</v>
+      <c r="F24" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="7" t="s">
@@ -1224,18 +1242,18 @@
       <c r="J24" s="1"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="11" t="s">
-        <v>58</v>
+      <c r="F25" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="7" t="s">
@@ -1247,21 +1265,79 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="5"/>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="H26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
-        <v>65</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Peticiones de listar clientes y mostrar detalles de uno
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666A954D-5C48-4727-819D-94A98A6848BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A5BC5-200E-4259-8252-E6F284B08589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,8 +836,8 @@
         <v>53</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="7" t="s">
-        <v>4</v>
+      <c r="H5" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="1" t="s">
@@ -1027,8 +1027,8 @@
         <v>54</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="7" t="s">
-        <v>4</v>
+      <c r="H14" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="1"/>

</xml_diff>

<commit_message>
Peticiones modificar cliente y borrar
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A5BC5-200E-4259-8252-E6F284B08589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A019F4-FDAA-486D-8393-150D79590508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -102,18 +102,12 @@
     <t>Como ADMIN, quiero eliminar un mecánico</t>
   </si>
   <si>
-    <t>Como ADMIN, quiero eliminar una cita</t>
-  </si>
-  <si>
     <t>Como ADMIN-MEC, quiero ver los detalles de un cliente</t>
   </si>
   <si>
     <t>Como ADMIN-MEC, quiero ver los detalles de una cita</t>
   </si>
   <si>
-    <t>Pedirá una cita en una fecha y hora que entre dentro de un límite (lunes-viernes, 8:00-16:30). Obligatorio subir imágenes del estado del vehículo y el cuenta km. No podrá escribir los servicios a aplicar. Se hará en otro endpoint en el que los datos del cliente se autorellenen con el cliente buscado por ID.</t>
-  </si>
-  <si>
     <t>Listado paginado y con posibilidad de filtrar por nombre o tlf</t>
   </si>
   <si>
@@ -147,24 +141,15 @@
     <t>HABITUAL =  Cliente login</t>
   </si>
   <si>
-    <t>ADMIN = Mecánico plenos poderes</t>
-  </si>
-  <si>
     <t>MEC = Mecánico normal</t>
   </si>
   <si>
-    <t>Cada endpoint implica controlador, validación, gestión de errores, seguridad, y pantalla en flutter</t>
-  </si>
-  <si>
     <t>Como OCASIONAL, quiero crear un nuevo usuario HABITUAL</t>
   </si>
   <si>
     <t>Se podrán cancelar las citas siempre y cuando no estén en Proceso/Terminada</t>
   </si>
   <si>
-    <t>Modificar fecha-hora o imágenes de la cita no puede estar Aceptada aún, no mostrar servicios</t>
-  </si>
-  <si>
     <t>Como ADMIN-MEC, quiero comentar en una cita</t>
   </si>
   <si>
@@ -235,6 +220,21 @@
   </si>
   <si>
     <t>Como ADMIN-MEC, quiero cambiar mi contraseña</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
+  </si>
+  <si>
+    <t>ADMIN = Mecánico administrador</t>
+  </si>
+  <si>
+    <t>Modificar fecha-hora o imágenes de la cita solo si está en Trámite, no mostrar servicios</t>
+  </si>
+  <si>
+    <t>Pedirá una cita en una fecha y hora que entre dentro de un límite (lunes-viernes, 8:00-16:30). Obligatorio subir imágenes del estado del vehículo y el cuenta km. No podrá escribir los servicios a aplicar. Se hará en otro endpoint en el que los datos del cliente se autorellenen con el cliente buscado por ID. Se creará directamente como Trámite</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero cancelar una cita</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,12 +276,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,11 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -364,15 +358,15 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,7 +397,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>597018</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -712,7 +706,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,11 +716,11 @@
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="95.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -740,10 +734,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
@@ -755,70 +749,70 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="5"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4"/>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -827,65 +821,63 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="K7" s="3"/>
     </row>
@@ -894,19 +886,19 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="K8" s="3"/>
     </row>
@@ -915,19 +907,19 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
     </row>
@@ -936,19 +928,19 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="4"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
     </row>
@@ -957,59 +949,59 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="K12" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
       <c r="K13" s="3"/>
     </row>
@@ -1018,19 +1010,19 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="1"/>
       <c r="K14" s="3"/>
     </row>
@@ -1039,19 +1031,19 @@
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="4"/>
       <c r="J15" s="1"/>
       <c r="K15" s="3"/>
     </row>
@@ -1060,164 +1052,164 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="1"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="1"/>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="1"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="5"/>
-      <c r="K20" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="4"/>
       <c r="J21" s="1"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="K22" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="3"/>
     </row>
@@ -1226,19 +1218,19 @@
       <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="3"/>
     </row>
@@ -1247,40 +1239,40 @@
       <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="3"/>
     </row>
@@ -1289,40 +1281,40 @@
       <c r="B27" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="3"/>
     </row>
@@ -1332,12 +1324,12 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nuevas peticiones en cliente y mecánico
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A019F4-FDAA-486D-8393-150D79590508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85192460-C9C1-4554-B9CB-4CC655515F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -33,18 +33,12 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>Como OCASIONAL, quiero pedir una cita</t>
-  </si>
-  <si>
     <t>EN CUENTA</t>
   </si>
   <si>
     <t>TO DO</t>
   </si>
   <si>
-    <t>LEYENDA</t>
-  </si>
-  <si>
     <t>Como HABITUAL, quiero pedir una cita</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Como HABITUAL, quiero modificar mis datos personales/usuario</t>
   </si>
   <si>
-    <t>No se creará un usuario, solo se guardarán su datos y no tendrá acceso a modificar la cita</t>
-  </si>
-  <si>
     <t>Como HABITUAL, quiero comentar en una cita</t>
   </si>
   <si>
@@ -99,15 +90,9 @@
     <t>Como ADMIN-MEC, quiero crear una cita</t>
   </si>
   <si>
-    <t>Como ADMIN, quiero eliminar un mecánico</t>
-  </si>
-  <si>
     <t>Como ADMIN-MEC, quiero ver los detalles de un cliente</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC, quiero ver los detalles de una cita</t>
-  </si>
-  <si>
     <t>Listado paginado y con posibilidad de filtrar por nombre o tlf</t>
   </si>
   <si>
@@ -135,15 +120,6 @@
     <t>Añadir comentarios a la cita siempre que esté Aceptada/Proceso</t>
   </si>
   <si>
-    <t>OCASIONAL = Cliente sin login</t>
-  </si>
-  <si>
-    <t>HABITUAL =  Cliente login</t>
-  </si>
-  <si>
-    <t>MEC = Mecánico normal</t>
-  </si>
-  <si>
     <t>Como OCASIONAL, quiero crear un nuevo usuario HABITUAL</t>
   </si>
   <si>
@@ -156,9 +132,6 @@
     <t>Se podrán comentar las citas siempre que su estado sea Aceptada/Proceso</t>
   </si>
   <si>
-    <t>Eliminar un mecánico pero no las citas en que ha intervenido, se pondrá como null y mostrará un "No asignado"</t>
-  </si>
-  <si>
     <t>Eliminar una cita siempre y cuando no esté Proceso/Terminada</t>
   </si>
   <si>
@@ -219,15 +192,6 @@
     <t>Como ADMIN-MEC, quiero ver los detalles personales</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC, quiero cambiar mi contraseña</t>
-  </si>
-  <si>
-    <t>PROGRESS</t>
-  </si>
-  <si>
-    <t>ADMIN = Mecánico administrador</t>
-  </si>
-  <si>
     <t>Modificar fecha-hora o imágenes de la cita solo si está en Trámite, no mostrar servicios</t>
   </si>
   <si>
@@ -235,13 +199,55 @@
   </si>
   <si>
     <t>Como ADMIN, quiero cancelar una cita</t>
+  </si>
+  <si>
+    <t>RUTA</t>
+  </si>
+  <si>
+    <t>/auth/cliente/{id}</t>
+  </si>
+  <si>
+    <t>/auth/mecanico/</t>
+  </si>
+  <si>
+    <t>/auth/cliente/</t>
+  </si>
+  <si>
+    <t>/auth/user/changePsw</t>
+  </si>
+  <si>
+    <t>/noauth/user/register</t>
+  </si>
+  <si>
+    <t>/noauth/user/login</t>
+  </si>
+  <si>
+    <t>/auth/mecanico/{id}</t>
+  </si>
+  <si>
+    <t>/auth/mecanico/admin</t>
+  </si>
+  <si>
+    <t>/auth/mecanico/mec</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero eliminar un mecánico o un admin</t>
+  </si>
+  <si>
+    <t>Eliminar un mecánico pero no las citas en que ha intervenido, se pondrá como null y mostrará un "No asignado". SOLO PODRÁ HACERLO UN ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>/auth/cliente/{id}/citas</t>
+  </si>
+  <si>
+    <t>Como HABITUAL-ADMIN-MEC, quiero ver los detalles de una cita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +267,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -311,7 +323,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -358,14 +370,13 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -395,10 +406,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>597018</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>13812</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -427,8 +438,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16678275" y="190500"/>
-          <a:ext cx="6073893" cy="7372350"/>
+          <a:off x="16725900" y="190500"/>
+          <a:ext cx="4881087" cy="5924550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -703,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,11 +742,11 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
@@ -743,593 +754,577 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="13" t="s">
-        <v>4</v>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="1" t="s">
-        <v>36</v>
+      <c r="J2" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="8" t="s">
-        <v>57</v>
+      <c r="H3" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="1" t="s">
-        <v>37</v>
+      <c r="J3" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="7" t="s">
-        <v>47</v>
+      <c r="F4" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="8" t="s">
-        <v>57</v>
+      <c r="H4" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="1" t="s">
-        <v>66</v>
+      <c r="J4" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="8" t="s">
-        <v>57</v>
+      <c r="H5" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="1" t="s">
-        <v>38</v>
+      <c r="J5" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
+      <c r="F6" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="14"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="7" t="s">
-        <v>47</v>
+      <c r="F7" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="9" t="s">
-        <v>51</v>
+      <c r="F8" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="10" t="s">
-        <v>52</v>
+      <c r="F9" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6" t="s">
-        <v>4</v>
+      <c r="H10" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="J10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="8" t="s">
-        <v>57</v>
+      <c r="H11" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I11" s="4"/>
+      <c r="J11" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="9" t="s">
-        <v>51</v>
+      <c r="F12" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="6" t="s">
-        <v>65</v>
+      <c r="H12" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="J12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="10" t="s">
-        <v>52</v>
+      <c r="F13" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="8" t="s">
-        <v>57</v>
+      <c r="H13" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="8" t="s">
-        <v>57</v>
+      <c r="H14" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="6" t="s">
-        <v>4</v>
+      <c r="H16" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="6" t="s">
-        <v>4</v>
+      <c r="H17" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="8" t="s">
-        <v>48</v>
+      <c r="F19" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="6" t="s">
-        <v>4</v>
+      <c r="H19" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="3"/>
+      <c r="J19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="6" t="s">
-        <v>4</v>
+      <c r="H20" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="J20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="6" t="s">
-        <v>4</v>
+      <c r="H22" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="7" t="s">
-        <v>47</v>
+      <c r="F23" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="9" t="s">
-        <v>51</v>
+      <c r="F24" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="1"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="9" t="s">
-        <v>51</v>
+      <c r="F25" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="6" t="s">
-        <v>4</v>
+      <c r="H25" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="7" t="s">
-        <v>53</v>
+      <c r="F26" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Peticiones listado y detalles de citas
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85192460-C9C1-4554-B9CB-4CC655515F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5B5E5F-D766-410D-8130-20FF4CECEA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>Como HABITUAL-ADMIN-MEC, quiero ver los detalles de una cita</t>
+  </si>
+  <si>
+    <t>/auth/cita/</t>
+  </si>
+  <si>
+    <t>/auth/cita/{id}</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1069,13 @@
         <v>40</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="6" t="s">
-        <v>3</v>
+      <c r="H15" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="13"/>
+      <c r="J15" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1130,11 +1138,13 @@
         <v>39</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="6" t="s">
-        <v>3</v>
+      <c r="H18" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="13"/>
+      <c r="J18" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Crear nueva cita validada
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5B5E5F-D766-410D-8130-20FF4CECEA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A46B04-9B90-45F9-943D-0BF764A43A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Añadir comentarios a la cita siempre que esté Aceptada/Proceso</t>
   </si>
   <si>
-    <t>Como OCASIONAL, quiero crear un nuevo usuario HABITUAL</t>
-  </si>
-  <si>
     <t>Se podrán cancelar las citas siempre y cuando no estén en Proceso/Terminada</t>
   </si>
   <si>
@@ -247,6 +244,18 @@
   </si>
   <si>
     <t>/auth/cita/{id}</t>
+  </si>
+  <si>
+    <t>Como HABITUAL, quiero ver todos los comentarios</t>
+  </si>
+  <si>
+    <t>Se podrán ver todos los comentarios, con algún dato de la cita</t>
+  </si>
+  <si>
+    <t>Como OCASIONAL-ADMIN-MEC, quiero crear un nuevo usuario HABITUAL</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +342,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -346,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +400,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,16 +424,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>13812</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>23337</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -444,7 +462,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16725900" y="190500"/>
+          <a:off x="16125825" y="0"/>
           <a:ext cx="4881087" cy="5924550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -720,16 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="95.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
@@ -752,7 +770,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
@@ -760,14 +778,14 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
@@ -775,38 +793,38 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -821,15 +839,15 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -840,19 +858,19 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -863,11 +881,11 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="6" t="s">
@@ -884,11 +902,11 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="6" t="s">
@@ -905,11 +923,11 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="6" t="s">
@@ -926,11 +944,11 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="6" t="s">
@@ -941,101 +959,98 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="9" t="s">
-        <v>42</v>
+      <c r="F10" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="11" t="s">
-        <v>48</v>
+      <c r="H10" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="13" t="s">
-        <v>62</v>
+      <c r="J11" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="10" t="s">
-        <v>43</v>
+      <c r="F12" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="J12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="8" t="s">
-        <v>40</v>
+      <c r="F13" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
@@ -1043,11 +1058,11 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="12" t="s">
@@ -1058,34 +1073,34 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="8" t="s">
@@ -1093,183 +1108,187 @@
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="6" t="s">
-        <v>3</v>
+      <c r="H21" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="13"/>
+      <c r="J21" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="9" t="s">
-        <v>42</v>
+      <c r="F22" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="11" t="s">
-        <v>48</v>
+      <c r="H22" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="12" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="6" t="s">
-        <v>3</v>
+      <c r="H23" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="13"/>
+      <c r="J23" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="7" t="s">
-        <v>44</v>
+      <c r="F24" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="6" t="s">
@@ -1279,62 +1298,83 @@
       <c r="J24" s="13"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="11" t="s">
-        <v>48</v>
+      <c r="H25" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="J25" s="13"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="6" t="s">
-        <v>3</v>
+      <c r="H26" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="13"/>
+      <c r="J26" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Peticiones crear y modificar cita desde vista mecánico
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A46B04-9B90-45F9-943D-0BF764A43A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9125B810-9837-44BC-A3C0-6162D25363CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Como HABITUAL, quiero modificar una cita</t>
   </si>
   <si>
-    <t>Como HABITUAL, quiero cancelar una cita</t>
-  </si>
-  <si>
     <t>Como HABITUAL, quiero ver el histórico completo de mis citas</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Añadir comentarios a la cita siempre que esté Aceptada/Proceso</t>
   </si>
   <si>
-    <t>Se podrán cancelar las citas siempre y cuando no estén en Proceso/Terminada</t>
-  </si>
-  <si>
     <t>Como ADMIN-MEC, quiero comentar en una cita</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>Pedirá una cita en una fecha y hora que entre dentro de un límite (lunes-viernes, 8:00-16:30). Obligatorio subir imágenes del estado del vehículo y el cuenta km. No podrá escribir los servicios a aplicar. Se hará en otro endpoint en el que los datos del cliente se autorellenen con el cliente buscado por ID. Se creará directamente como Trámite</t>
   </si>
   <si>
-    <t>Como ADMIN, quiero cancelar una cita</t>
-  </si>
-  <si>
     <t>RUTA</t>
   </si>
   <si>
@@ -255,7 +246,10 @@
     <t>Como OCASIONAL-ADMIN-MEC, quiero crear un nuevo usuario HABITUAL</t>
   </si>
   <si>
-    <t>PROGRESS</t>
+    <t>Como ADMIN-MEC-HABITUAL, quiero cancelar una cita</t>
+  </si>
+  <si>
+    <t>/auth/cita/mecanico/{id}</t>
   </si>
 </sst>
 </file>
@@ -293,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,12 +336,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -361,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -399,9 +387,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +755,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
@@ -778,99 +763,99 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -881,11 +866,11 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="6" t="s">
@@ -902,11 +887,11 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="6" t="s">
@@ -919,15 +904,15 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="10" t="s">
-        <v>42</v>
+      <c r="F8" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="6" t="s">
@@ -938,65 +923,67 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="7" t="s">
-        <v>43</v>
+      <c r="F9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="6" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="8" t="s">
-        <v>38</v>
+      <c r="F10" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6" t="s">
-        <v>3</v>
+      <c r="H10" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="I10" s="4"/>
+      <c r="J10" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="13" t="s">
         <v>58</v>
       </c>
       <c r="K11" s="4"/>
@@ -1004,46 +991,46 @@
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="9" t="s">
-        <v>41</v>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="J12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="10" t="s">
-        <v>42</v>
+      <c r="F13" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" s="3"/>
     </row>
@@ -1054,19 +1041,19 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K14" s="3"/>
     </row>
@@ -1081,22 +1068,22 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="12" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
@@ -1104,114 +1091,114 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="12" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="12" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="8" t="s">
-        <v>38</v>
+      <c r="F19" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K19" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
@@ -1219,75 +1206,75 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="12" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="7" t="s">
-        <v>37</v>
+      <c r="F22" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="14" t="s">
-        <v>76</v>
+      <c r="H22" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="12" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G24" s="4"/>
@@ -1298,83 +1285,64 @@
       <c r="J24" s="13"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="7" t="s">
-        <v>43</v>
+      <c r="F25" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="6" t="s">
-        <v>3</v>
+      <c r="H25" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="13"/>
+      <c r="J25" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Petición crear y modificar cita desde vista cliente, y petición nuevo mensaje en chat
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9125B810-9837-44BC-A3C0-6162D25363CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5387EE-0262-4FAA-AAF4-2E80642224DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -36,9 +36,6 @@
     <t>EN CUENTA</t>
   </si>
   <si>
-    <t>TO DO</t>
-  </si>
-  <si>
     <t>Como HABITUAL, quiero pedir una cita</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Como HABITUAL, quiero modificar mis datos personales/usuario</t>
   </si>
   <si>
-    <t>Como HABITUAL, quiero comentar en una cita</t>
-  </si>
-  <si>
     <t>Modificar nombre, usuario, contraseña, email, tlf, ¿marca, modelo, matrícula?</t>
   </si>
   <si>
@@ -114,15 +108,6 @@
     <t>Modificar datos de un mecánico ya existente, solo nombre, usuario, email</t>
   </si>
   <si>
-    <t>Añadir comentarios a la cita siempre que esté Aceptada/Proceso</t>
-  </si>
-  <si>
-    <t>Como ADMIN-MEC, quiero comentar en una cita</t>
-  </si>
-  <si>
-    <t>Se podrán comentar las citas siempre que su estado sea Aceptada/Proceso</t>
-  </si>
-  <si>
     <t>Eliminar una cita siempre y cuando no esté Proceso/Terminada</t>
   </si>
   <si>
@@ -150,9 +135,6 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>POST/PUT</t>
-  </si>
-  <si>
     <t>Como HABITUAL, quiero darme de baja</t>
   </si>
   <si>
@@ -186,9 +168,6 @@
     <t>Modificar fecha-hora o imágenes de la cita solo si está en Trámite, no mostrar servicios</t>
   </si>
   <si>
-    <t>Pedirá una cita en una fecha y hora que entre dentro de un límite (lunes-viernes, 8:00-16:30). Obligatorio subir imágenes del estado del vehículo y el cuenta km. No podrá escribir los servicios a aplicar. Se hará en otro endpoint en el que los datos del cliente se autorellenen con el cliente buscado por ID. Se creará directamente como Trámite</t>
-  </si>
-  <si>
     <t>RUTA</t>
   </si>
   <si>
@@ -237,12 +216,6 @@
     <t>/auth/cita/{id}</t>
   </si>
   <si>
-    <t>Como HABITUAL, quiero ver todos los comentarios</t>
-  </si>
-  <si>
-    <t>Se podrán ver todos los comentarios, con algún dato de la cita</t>
-  </si>
-  <si>
     <t>Como OCASIONAL-ADMIN-MEC, quiero crear un nuevo usuario HABITUAL</t>
   </si>
   <si>
@@ -250,6 +223,21 @@
   </si>
   <si>
     <t>/auth/cita/mecanico/{id}</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC-HABITUAL, quiero comentar en una cita</t>
+  </si>
+  <si>
+    <t>Añadir comentarios a la cita siempre que esté Aceptada/Proceso. Se comentará en la propia</t>
+  </si>
+  <si>
+    <t>Pedirá una cita en una fecha y hora que entre dentro de un límite, subiendo imagenes del estado del vehículo y el cuenta km. Se autorellenan con el cliente buscado por ID. Se creará directamente como Trámite</t>
+  </si>
+  <si>
+    <t>/auth/cita/cliente/{id}</t>
+  </si>
+  <si>
+    <t>/auth/cita/cliente/{idCliente}/{idCita}</t>
   </si>
 </sst>
 </file>
@@ -287,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,12 +285,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -377,9 +359,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -723,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +719,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -755,7 +734,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
@@ -763,251 +742,260 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="7" t="s">
-        <v>35</v>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="11" t="s">
-        <v>45</v>
+      <c r="H2" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="12" t="s">
-        <v>59</v>
+      <c r="J2" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="11" t="s">
-        <v>45</v>
+      <c r="H3" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="12" t="s">
-        <v>60</v>
+      <c r="J3" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="8" t="s">
-        <v>36</v>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="11" t="s">
-        <v>45</v>
+      <c r="H4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="12" t="s">
-        <v>55</v>
+      <c r="J4" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="8" t="s">
-        <v>36</v>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="11" t="s">
-        <v>45</v>
+      <c r="H5" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="12" t="s">
-        <v>66</v>
+      <c r="J5" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="7" t="s">
-        <v>35</v>
+      <c r="F6" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6" t="s">
-        <v>3</v>
+      <c r="H6" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="9" t="s">
-        <v>39</v>
+      <c r="F7" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="6" t="s">
-        <v>3</v>
+      <c r="H7" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="13"/>
+      <c r="J7" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="7" t="s">
-        <v>41</v>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="6" t="s">
-        <v>3</v>
+      <c r="H8" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
         <v>36</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" t="s">
-        <v>7</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="11" t="s">
-        <v>45</v>
+      <c r="H10" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="J10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="10" t="s">
-        <v>40</v>
+      <c r="F12" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="11" t="s">
-        <v>45</v>
+      <c r="H12" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="12" t="s">
-        <v>55</v>
+      <c r="J12" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="K12" s="3"/>
     </row>
@@ -1018,331 +1006,285 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="8" t="s">
-        <v>37</v>
+      <c r="F13" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="11" t="s">
-        <v>45</v>
+      <c r="H13" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="12" t="s">
-        <v>57</v>
+      <c r="J13" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="8" t="s">
-        <v>37</v>
+      <c r="F14" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="11" t="s">
-        <v>45</v>
+      <c r="H14" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="12" t="s">
-        <v>56</v>
+      <c r="J14" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="8" t="s">
-        <v>37</v>
+      <c r="F15" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="11" t="s">
-        <v>45</v>
+      <c r="H15" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="12" t="s">
-        <v>68</v>
+      <c r="J15" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="8" t="s">
-        <v>36</v>
+      <c r="F16" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="11" t="s">
-        <v>45</v>
+      <c r="H16" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="12" t="s">
-        <v>55</v>
+      <c r="J16" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="8" t="s">
-        <v>36</v>
+      <c r="F17" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="11" t="s">
-        <v>45</v>
+      <c r="H17" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K17" s="3"/>
+      <c r="J17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="8" t="s">
-        <v>36</v>
+      <c r="F18" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="11" t="s">
-        <v>45</v>
+      <c r="H18" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="12" t="s">
-        <v>69</v>
+      <c r="J18" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="7" t="s">
-        <v>35</v>
+      <c r="F19" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="11" t="s">
-        <v>45</v>
+      <c r="H19" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K19" s="4"/>
+      <c r="J19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="7" t="s">
-        <v>35</v>
+      <c r="F20" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="11" t="s">
-        <v>45</v>
+      <c r="H20" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="12" t="s">
-        <v>63</v>
+      <c r="J20" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="7" t="s">
-        <v>35</v>
+      <c r="F21" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="11" t="s">
-        <v>45</v>
+      <c r="H21" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="12" t="s">
-        <v>74</v>
+      <c r="J21" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="9" t="s">
-        <v>39</v>
+      <c r="F22" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="11" t="s">
-        <v>45</v>
+      <c r="H22" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="12" t="s">
-        <v>61</v>
-      </c>
+      <c r="J22" s="12"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="11" t="s">
-        <v>45</v>
+      <c r="H23" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="12" t="s">
-        <v>74</v>
+      <c r="J23" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="7" t="s">
-        <v>41</v>
+      <c r="F24" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="6" t="s">
-        <v>3</v>
+      <c r="H24" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="13"/>
+      <c r="J24" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementación autenticación en peticiones de cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5387EE-0262-4FAA-AAF4-2E80642224DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BE9167-69AD-4CAC-A610-49B4354C2048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Modificar nombre, usuario, contraseña, email, tlf, ¿marca, modelo, matrícula?</t>
   </si>
   <si>
-    <t>Como ADMIN, quiero modificar los datos de un mecánico</t>
-  </si>
-  <si>
     <t>Se hará desde la pantalla principal antes de loguearse</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Eliminar el cliente pero no sus citas, se dejarán con el cliente a null y se mostrará su nombre y apellidos. Solo podrá borrarse a sí mismo</t>
   </si>
   <si>
-    <t>Como HABITUAL, quiero modificar mi contraseña</t>
-  </si>
-  <si>
     <t>Obligatorio poner la antigua para comprobar que está bien, y dos veces la nueva que no coincida con antigua</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>Eliminar un mecánico pero no las citas en que ha intervenido, se pondrá como null y mostrará un "No asignado". SOLO PODRÁ HACERLO UN ADMINISTRADOR</t>
   </si>
   <si>
-    <t>/auth/cliente/{id}/citas</t>
-  </si>
-  <si>
     <t>Como HABITUAL-ADMIN-MEC, quiero ver los detalles de una cita</t>
   </si>
   <si>
@@ -237,14 +228,47 @@
     <t>/auth/cita/cliente/{id}</t>
   </si>
   <si>
-    <t>/auth/cita/cliente/{idCliente}/{idCita}</t>
+    <t>Como ADMIN, MEC, HABITUAL, quiero modificar mi contraseña</t>
+  </si>
+  <si>
+    <t>ADMIN: mrl26 / admin1234</t>
+  </si>
+  <si>
+    <t>MEC: asp14 / mec1234</t>
+  </si>
+  <si>
+    <t>CLIENTE: jjml4 / cli1234</t>
+  </si>
+  <si>
+    <t>AUTH</t>
+  </si>
+  <si>
+    <t>/auth/cliente/me/citas</t>
+  </si>
+  <si>
+    <t>/auth/cita/cliente</t>
+  </si>
+  <si>
+    <t>MODIFICAR CITA, QUE SE PUEDA DEJAR LA MISMA FECHA, PARA QUE NO HAYA QUE CAMBIARLA SIEMPRE (AUTH/CITA/CLIENTE/IDCITA</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero modificar los datos de un mecánico o un admin</t>
+  </si>
+  <si>
+    <t>/auth/cliente/me</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero eliminar un usuario</t>
+  </si>
+  <si>
+    <t>Eliminar un cliente por su ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,8 +298,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,7 +345,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -358,13 +395,20 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -702,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +761,7 @@
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
     <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
@@ -734,7 +778,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
@@ -742,76 +786,76 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="10" t="s">
-        <v>39</v>
+      <c r="H2" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="11" t="s">
-        <v>52</v>
+      <c r="J2" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="10" t="s">
-        <v>39</v>
+      <c r="H3" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="11" t="s">
-        <v>53</v>
+      <c r="J3" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="10" t="s">
-        <v>39</v>
+      <c r="H4" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="11" t="s">
-        <v>48</v>
+      <c r="J4" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -822,19 +866,19 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="10" t="s">
-        <v>39</v>
+      <c r="H5" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="11" t="s">
-        <v>59</v>
+      <c r="J5" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -845,19 +889,19 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="10" t="s">
-        <v>39</v>
+      <c r="H6" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="11" t="s">
-        <v>69</v>
+      <c r="J6" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -868,19 +912,19 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="10" t="s">
-        <v>39</v>
+      <c r="H7" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="11" t="s">
-        <v>70</v>
+      <c r="J7" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="K7" s="3"/>
     </row>
@@ -895,396 +939,439 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="10" t="s">
-        <v>39</v>
+      <c r="H8" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="11" t="s">
-        <v>48</v>
+      <c r="J8" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="10" t="s">
-        <v>39</v>
+      <c r="H9" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="12" t="s">
-        <v>51</v>
+      <c r="J9" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="10" t="s">
-        <v>39</v>
+      <c r="H10" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="11" t="s">
-        <v>48</v>
+      <c r="J10" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="10" t="s">
-        <v>39</v>
+      <c r="H11" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="11" t="s">
-        <v>50</v>
+      <c r="J11" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="10" t="s">
-        <v>39</v>
+      <c r="H12" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="11" t="s">
-        <v>49</v>
+      <c r="J12" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="10" t="s">
-        <v>39</v>
+      <c r="H13" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="11" t="s">
-        <v>61</v>
+      <c r="J13" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="10" t="s">
-        <v>39</v>
+      <c r="H14" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="11" t="s">
-        <v>48</v>
+      <c r="J14" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="10" t="s">
-        <v>39</v>
+      <c r="H15" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="11" t="s">
-        <v>54</v>
+      <c r="J15" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="10" t="s">
-        <v>39</v>
+      <c r="H16" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="11" t="s">
-        <v>62</v>
+      <c r="J16" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="10" t="s">
-        <v>39</v>
+      <c r="H17" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="11" t="s">
-        <v>55</v>
+      <c r="J17" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="10" t="s">
-        <v>39</v>
+      <c r="H18" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="11" t="s">
-        <v>56</v>
+      <c r="J18" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="10" t="s">
-        <v>39</v>
+      <c r="H19" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="11" t="s">
-        <v>65</v>
+      <c r="J19" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="10" t="s">
-        <v>39</v>
+      <c r="H20" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="11" t="s">
-        <v>54</v>
+      <c r="J20" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="10" t="s">
-        <v>39</v>
+      <c r="H21" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="11" t="s">
-        <v>65</v>
+      <c r="J21" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="10" t="s">
-        <v>39</v>
+      <c r="H22" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="11"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="10" t="s">
-        <v>39</v>
+      <c r="H23" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="11" t="s">
-        <v>54</v>
+      <c r="J23" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="10" t="s">
-        <v>39</v>
+      <c r="H24" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K24" s="3"/>
+      <c r="J24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="H25" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D27" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementación autorización para rol MEC y ADMIN de peticiones de cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BE9167-69AD-4CAC-A610-49B4354C2048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC8A805-ACBF-4C69-A69E-0BDFABA7CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,10 +258,10 @@
     <t>/auth/cliente/me</t>
   </si>
   <si>
-    <t>Como ADMIN, quiero eliminar un usuario</t>
-  </si>
-  <si>
     <t>Eliminar un cliente por su ID</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero eliminar un cliente</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,8 +1011,8 @@
         <v>31</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="12" t="s">
-        <v>71</v>
+      <c r="H11" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="10" t="s">
@@ -1080,8 +1080,8 @@
         <v>30</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="12" t="s">
-        <v>71</v>
+      <c r="H14" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="10" t="s">
@@ -1297,19 +1297,19 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="12" t="s">
-        <v>71</v>
+      <c r="H24" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="10" t="s">

</xml_diff>

<commit_message>
Implementación autorización peticiones mecánicos y citas para rol ADMIN, MEC
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC8A805-ACBF-4C69-A69E-0BDFABA7CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3B234A-718A-4A39-916A-505F998A8625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Obligatorio poner la antigua para comprobar que está bien, y dos veces la nueva que no coincida con antigua</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC, quiero ver los detalles personales</t>
-  </si>
-  <si>
     <t>Modificar fecha-hora o imágenes de la cita solo si está en Trámite, no mostrar servicios</t>
   </si>
   <si>
@@ -262,6 +259,27 @@
   </si>
   <si>
     <t>Como ADMIN, quiero eliminar un cliente</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC-HABITUAL quiero modificar mi foto de perfil</t>
+  </si>
+  <si>
+    <t>/auth/mecanico/me</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC quiero ver los detalles de un mecánico o admin</t>
+  </si>
+  <si>
+    <t>Como ADMIN, quiero ver los detalles de un mecánico o admin</t>
+  </si>
+  <si>
+    <t>Página de detalles del mecánico</t>
+  </si>
+  <si>
+    <t>/auth/user/avatar</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -368,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -411,6 +429,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +462,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>23337</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -746,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,13 +778,13 @@
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="95.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -786,14 +807,14 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
@@ -809,7 +830,7 @@
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="3"/>
     </row>
@@ -832,7 +853,7 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -855,7 +876,7 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -878,7 +899,7 @@
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K5" s="3"/>
     </row>
@@ -889,7 +910,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6" t="s">
@@ -901,7 +922,7 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -912,7 +933,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="8" t="s">
@@ -924,7 +945,7 @@
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" s="3"/>
     </row>
@@ -947,14 +968,14 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
@@ -970,7 +991,7 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" s="4"/>
     </row>
@@ -993,7 +1014,7 @@
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K10" s="3"/>
     </row>
@@ -1016,68 +1037,65 @@
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="7" t="s">
-        <v>31</v>
+      <c r="F12" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="12" t="s">
-        <v>71</v>
+      <c r="H12" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="12" t="s">
-        <v>71</v>
+      <c r="H13" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="7" t="s">
@@ -1085,110 +1103,110 @@
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="10" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="12" t="s">
-        <v>71</v>
+      <c r="H15" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="12" t="s">
-        <v>71</v>
+      <c r="H16" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K16" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="6" t="s">
-        <v>29</v>
+      <c r="F17" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="12" t="s">
-        <v>71</v>
+      <c r="H17" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="6" t="s">
-        <v>29</v>
+      <c r="F18" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="12" t="s">
-        <v>71</v>
+      <c r="H18" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
@@ -1196,135 +1214,135 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K19" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="8" t="s">
-        <v>33</v>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="8" t="s">
-        <v>33</v>
+      <c r="F21" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="6" t="s">
-        <v>29</v>
+      <c r="F22" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="11"/>
+      <c r="J22" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="9" t="s">
-        <v>34</v>
+      <c r="F23" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="9" t="s">
-        <v>34</v>
+      <c r="F24" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="7" t="s">
-        <v>38</v>
+      <c r="H24" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="11"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="9" t="s">
@@ -1332,45 +1350,91 @@
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="4"/>
+      <c r="H26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D27" s="15" t="s">
-        <v>74</v>
-      </c>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reestructuración código y carpetas
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E423384F-8272-4B7F-A030-6E002D6F0788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66970868-D257-4BD2-B6D6-B9132103ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Como ADMIN-MEC-HABITUAL, quiero hacer logout</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -264,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +310,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -320,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -347,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,8 +784,8 @@
         <v>16</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
+      <c r="F4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">

</xml_diff>

<commit_message>
Implementación detalles cliente logueado
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66970868-D257-4BD2-B6D6-B9132103ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B88C4E-2DB0-4785-8B54-D54C3EFE13AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,22 +383,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>524802</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>429849</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3FD593-7F8C-55B7-5960-9DD2C1FB742C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{596D2324-8DA3-D2E2-A811-E0B78384DF20}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -420,8 +420,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9229724" y="0"/>
-          <a:ext cx="4896778" cy="5734050"/>
+          <a:off x="9353550" y="0"/>
+          <a:ext cx="5411424" cy="6105525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,8 +784,8 @@
         <v>16</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="12" t="s">
-        <v>65</v>
+      <c r="F4" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
@@ -803,8 +803,8 @@
         <v>16</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="4" t="s">
-        <v>22</v>
+      <c r="F5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">

</xml_diff>

<commit_message>
Termino implementación citas cliente logueado
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B88C4E-2DB0-4785-8B54-D54C3EFE13AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48669F33-9A9C-45AA-8CA0-267A81ABAA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,8 +803,8 @@
         <v>16</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="12" t="s">
-        <v>65</v>
+      <c r="F5" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">
@@ -1050,8 +1050,8 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="4" t="s">
-        <v>22</v>
+      <c r="F18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">

</xml_diff>

<commit_message>
Implementación detalles de una cita y su chat
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48669F33-9A9C-45AA-8CA0-267A81ABAA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491746D6-15E7-4C1F-B6D9-EF8FB0E944F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,8 +822,8 @@
         <v>15</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
+      <c r="F6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">
@@ -1050,8 +1050,8 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="12" t="s">
-        <v>65</v>
+      <c r="F18" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
@@ -1297,8 +1297,8 @@
         <v>15</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="4" t="s">
-        <v>22</v>
+      <c r="F31" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
Implementación pedir nueva cita
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491746D6-15E7-4C1F-B6D9-EF8FB0E944F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B33286C-D381-4F8E-9531-CE9EDCDA07EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,8 +1297,8 @@
         <v>15</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="12" t="s">
-        <v>65</v>
+      <c r="F31" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
Implementación pedir cita cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B33286C-D381-4F8E-9531-CE9EDCDA07EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5382236F-F924-4C98-B962-51119C777F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>Como ADMIN-MEC-HABITUAL, quiero hacer logout</t>
-  </si>
-  <si>
-    <t>PROGRESS</t>
   </si>
 </sst>
 </file>
@@ -267,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,12 +307,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -356,9 +347,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,7 +687,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,8 +810,8 @@
         <v>15</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="12" t="s">
-        <v>65</v>
+      <c r="F6" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">

</xml_diff>

<commit_message>
Implementación modificar una cita
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14644D4-E326-4ED9-A744-27C0804DF6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52B1E98-F5B3-4A61-BFA0-164341BAC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,8 +841,8 @@
         <v>18</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="4" t="s">
-        <v>22</v>
+      <c r="F7" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
@@ -860,8 +860,8 @@
         <v>18</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="12" t="s">
-        <v>65</v>
+      <c r="F8" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="9" t="s">
@@ -879,8 +879,8 @@
         <v>18</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
+      <c r="F9" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="10" t="s">

</xml_diff>

<commit_message>
Implementación modificar contraseña usuario
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52B1E98-F5B3-4A61-BFA0-164341BAC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C84D4E-2FD2-4EC1-B6EF-9BE60CD3F7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,8 +879,8 @@
         <v>18</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="12" t="s">
-        <v>65</v>
+      <c r="F9" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="10" t="s">
@@ -898,8 +898,8 @@
         <v>19</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="4" t="s">
-        <v>22</v>
+      <c r="F10" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">

</xml_diff>

<commit_message>
Implementación borrar cliente y cancelar cita cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C84D4E-2FD2-4EC1-B6EF-9BE60CD3F7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E81459-E2FD-482E-8F77-31F1DD57677E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -183,9 +183,6 @@
     <t>/auth/mecanico/me</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC quiero ver los detalles de un mecánico o admin</t>
-  </si>
-  <si>
     <t>Como ADMIN, quiero ver los detalles de un mecánico o admin</t>
   </si>
   <si>
@@ -222,7 +219,7 @@
     <t>Como ADMIN-MEC-HABITUAL, quiero hacer logout</t>
   </si>
   <si>
-    <t>PROGRESS</t>
+    <t>Como ADMIN-MEC quiero ver mis detalles de un mecánico o admin</t>
   </si>
 </sst>
 </file>
@@ -267,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,12 +307,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -356,9 +347,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,7 +687,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +735,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="9" t="s">
@@ -766,7 +754,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="9" t="s">
@@ -785,7 +773,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
@@ -804,7 +792,7 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">
@@ -823,7 +811,7 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">
@@ -842,11 +830,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -861,7 +849,7 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="9" t="s">
@@ -880,7 +868,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="10" t="s">
@@ -898,8 +886,8 @@
         <v>19</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="12" t="s">
-        <v>65</v>
+      <c r="F10" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">
@@ -910,19 +898,19 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="4" t="s">
-        <v>22</v>
+      <c r="F11" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1005,7 +993,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="4" t="s">
@@ -1024,7 +1012,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="4" t="s">
@@ -1051,7 +1039,7 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
@@ -1169,7 +1157,7 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1214,7 +1202,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="6" t="s">
@@ -1245,14 +1233,14 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="3" t="s">
@@ -1264,14 +1252,14 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="6" t="s">
@@ -1283,14 +1271,14 @@
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="3" t="s">
@@ -1298,7 +1286,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
Solución problemas lista infinita
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF3091D-755D-4F62-9C62-76FB790D3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B06FA4-5573-4782-B68B-C6725F0BE56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,8 +936,8 @@
         <v>17</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="12" t="s">
-        <v>65</v>
+      <c r="F12" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="9" t="s">
@@ -955,8 +955,8 @@
         <v>17</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="4" t="s">
-        <v>22</v>
+      <c r="F13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">

</xml_diff>

<commit_message>
Implementación listado mecánicos y citas
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B06FA4-5573-4782-B68B-C6725F0BE56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A706225-1004-4B1A-814C-F44A05CC8CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,8 +955,8 @@
         <v>17</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="12" t="s">
-        <v>65</v>
+      <c r="F13" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">
@@ -974,8 +974,8 @@
         <v>17</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="4" t="s">
-        <v>22</v>
+      <c r="F14" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="9" t="s">
@@ -993,8 +993,8 @@
         <v>16</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="4" t="s">
-        <v>22</v>
+      <c r="F15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="s">
@@ -1050,7 +1050,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="12" t="s">
         <v>62</v>
       </c>
       <c r="G18" s="1"/>

</xml_diff>

<commit_message>
Implementación detalles clientes, mecánicos y citas
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A706225-1004-4B1A-814C-F44A05CC8CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADC5BAE-D295-4179-AB62-C9D85AC5B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>PROGRESS</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -359,6 +368,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,7 +711,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,8 +1005,8 @@
         <v>16</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="12" t="s">
-        <v>65</v>
+      <c r="F15" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="s">
@@ -1012,8 +1024,8 @@
         <v>16</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="4" t="s">
-        <v>22</v>
+      <c r="F16" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="9" t="s">
@@ -1050,7 +1062,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G18" s="1"/>
@@ -1069,8 +1081,8 @@
         <v>15</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="4" t="s">
-        <v>22</v>
+      <c r="F19" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="s">
@@ -1293,8 +1305,8 @@
         <v>63</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="3" t="s">
-        <v>15</v>
+      <c r="D31" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11" t="s">

</xml_diff>

<commit_message>
Implementación nuevo administrador y nuevo mecánico
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADC5BAE-D295-4179-AB62-C9D85AC5B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BF5D7D-0AC3-4207-813E-F39A8BE2C307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Los del admin propio se modifican en el drawer del menu ppal, y los de un mecánico en la lista de mecánico en los detalles del que sea</t>
   </si>
 </sst>
 </file>
@@ -338,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -373,6 +376,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +715,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,8 +1085,8 @@
         <v>15</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="12" t="s">
-        <v>65</v>
+      <c r="F19" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="s">
@@ -1100,8 +1104,8 @@
         <v>15</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="4" t="s">
-        <v>22</v>
+      <c r="F20" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9" t="s">
@@ -1119,8 +1123,8 @@
         <v>15</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="4" t="s">
-        <v>22</v>
+      <c r="F21" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="s">
@@ -1138,7 +1142,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="1"/>
@@ -1326,17 +1330,21 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F33" s="14"/>
+      <c r="H33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Implementación nueva cita vista mecánico y modificar mecánico
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BF5D7D-0AC3-4207-813E-F39A8BE2C307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340C4DD3-EB96-4F8C-8357-F5BF8C80C66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -222,13 +222,7 @@
     <t>Como ADMIN-MEC quiero ver mis detalles de un mecánico o admin</t>
   </si>
   <si>
-    <t>PROGRESS</t>
-  </si>
-  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Los del admin propio se modifican en el drawer del menu ppal, y los de un mecánico en la lista de mecánico en los detalles del que sea</t>
   </si>
 </sst>
 </file>
@@ -273,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,12 +312,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -341,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -373,10 +361,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +700,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,8 +1108,8 @@
         <v>15</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="12" t="s">
-        <v>65</v>
+      <c r="F21" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="s">
@@ -1142,8 +1127,8 @@
         <v>18</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="6" t="s">
-        <v>22</v>
+      <c r="F22" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9" t="s">
@@ -1309,8 +1294,8 @@
         <v>63</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="13" t="s">
-        <v>66</v>
+      <c r="D31" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11" t="s">
@@ -1330,21 +1315,18 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="H33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Implementación modificar cita vista cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340C4DD3-EB96-4F8C-8357-F5BF8C80C66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A925FD03-A234-4272-9EEE-6362D8953FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>PROGRESS</t>
+  </si>
+  <si>
+    <t>METER TODOS LOS SCREEN EN UN SCROLLVIEW, PROBAR LAS PANTALLAS PARA QUE EL LARGO HAGA SCROLL Y NO PETE</t>
+  </si>
+  <si>
+    <t>COMPROBAR QUE SE PUEDE NAVEGAR A OTROS SITIOS DESDE MODIFICAR CITA MECANICO</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +325,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -329,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -361,7 +382,11 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,8 +1171,8 @@
         <v>18</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="4" t="s">
-        <v>22</v>
+      <c r="F23" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
@@ -1315,20 +1340,28 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="14"/>
+      <c r="H36" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección modificar cita vista cliente
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A925FD03-A234-4272-9EEE-6362D8953FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491F510D-97F1-4CFC-B627-DF0BEE6C66B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,7 +231,7 @@
     <t>METER TODOS LOS SCREEN EN UN SCROLLVIEW, PROBAR LAS PANTALLAS PARA QUE EL LARGO HAGA SCROLL Y NO PETE</t>
   </si>
   <si>
-    <t>COMPROBAR QUE SE PUEDE NAVEGAR A OTROS SITIOS DESDE MODIFICAR CITA MECANICO</t>
+    <t>PASAR A PROD APPLICATIONPROPERTIES</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,12 +331,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -350,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -386,7 +380,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,7 +720,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,8 +1166,8 @@
         <v>18</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="13" t="s">
-        <v>66</v>
+      <c r="F23" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
@@ -1190,8 +1185,8 @@
         <v>15</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="4" t="s">
-        <v>22</v>
+      <c r="F24" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="10" t="s">
@@ -1344,6 +1339,9 @@
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="H33" s="15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
@@ -1359,10 +1357,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="14"/>
-      <c r="H36" s="15" t="s">
-        <v>68</v>
-      </c>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mejoras en diseño de formularios
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9138F9-A47B-4CFD-A367-67F3655BF411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082964AF-67C8-4ED0-A866-1FA5E0E24C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -228,13 +228,13 @@
     <t>PROGRESS</t>
   </si>
   <si>
-    <t>METER TODOS LOS SCREEN EN UN SCROLLVIEW, PROBAR LAS PANTALLAS PARA QUE EL LARGO HAGA SCROLL Y NO PETE</t>
-  </si>
-  <si>
     <t>PASAR A PROD APPLICATIONPROPERTIES</t>
   </si>
   <si>
-    <t>LA PANTALLA DE ME-LOGIN SE CORTA, METERLO EN UN CONTAINER Y LUEGO UN SCROLLVIEW</t>
+    <t>No borrar usuarios, solo desactivarlos (enabled = false) en caso de ser un cliente con citas, y en cualquier caso de los mecánicos/admin, y para los clientes sin cita, si borrarlos. Luego, para el login, comprobar en el servidor si enables = true para que deje loguearse, y si no crear una excepción que diga que el usuario está desactivado.</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +334,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -347,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -382,8 +388,14 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1085,8 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="11" t="s">
-        <v>62</v>
+      <c r="F18" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
@@ -1187,8 +1199,8 @@
         <v>15</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="13" t="s">
-        <v>66</v>
+      <c r="F24" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="10" t="s">
@@ -1206,8 +1218,8 @@
         <v>19</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="4" t="s">
-        <v>22</v>
+      <c r="F25" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="9" t="s">
@@ -1341,24 +1353,26 @@
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H33" s="15" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H35" t="s">
-        <v>69</v>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación métodos borrado cliente y mecánico en vista mecánico
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082964AF-67C8-4ED0-A866-1FA5E0E24C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D443F621-3268-40B3-9781-CE8B9BDBDC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>No borrar usuarios, solo desactivarlos (enabled = false) en caso de ser un cliente con citas, y en cualquier caso de los mecánicos/admin, y para los clientes sin cita, si borrarlos. Luego, para el login, comprobar en el servidor si enables = true para que deje loguearse, y si no crear una excepción que diga que el usuario está desactivado.</t>
-  </si>
-  <si>
-    <t>REVISAR</t>
   </si>
 </sst>
 </file>
@@ -279,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,12 +331,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -353,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -389,12 +380,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,7 +721,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,8 +920,8 @@
         <v>19</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="11" t="s">
-        <v>62</v>
+      <c r="F10" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">
@@ -1085,8 +1072,8 @@
         <v>16</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="17" t="s">
-        <v>69</v>
+      <c r="F18" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
@@ -1237,8 +1224,8 @@
         <v>19</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="4" t="s">
-        <v>22</v>
+      <c r="F26" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="9" t="s">
@@ -1256,8 +1243,8 @@
         <v>19</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
+      <c r="F27" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="9" t="s">
@@ -1349,29 +1336,28 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
+    <row r="37" spans="2:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección errores para ficheros y guardado fotos de perfil de cada usuario
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70869DB-78B2-4792-96B3-CF6939D1A639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E042414D-AA60-44FB-B3A3-2C526DF63498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -231,7 +231,19 @@
     <t>PASAR A PROD APPLICATIONPROPERTIES</t>
   </si>
   <si>
-    <t>SI SE ELIMINA UNA CITA EN TRÁMITE O ACEPTADA SE BORRAN LOS ADJUNTOS???</t>
+    <t>SI SE ELIMINA UNA CITA EN TRÁMITE O ACEPTADA SE BORRAN LOS ADJUNTOS, Y SI HAY FOTOS, LAS QUE ESTÉN EN LA CARPETA???</t>
+  </si>
+  <si>
+    <t>README + SWAGGER + COLECCIÓN POSTMAN</t>
+  </si>
+  <si>
+    <t>BORRAR TODO PARA VER QUE NO PETA</t>
+  </si>
+  <si>
+    <t>BUSCAR FOTO QUE NO EXISTE PARA TRATAR EL ERROR</t>
+  </si>
+  <si>
+    <t>SI HAGO POST DE FICHERO SIN METER NADA, DA ERROR 500, PUEDE SER PORQUE LLAMO A FILESTORAGESYSTEM Y NO A STORAGE SERVICE. MIRAR EJEMPLO LUISMI</t>
   </si>
 </sst>
 </file>
@@ -276,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +343,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -379,13 +397,11 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,16 +1371,33 @@
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="16"/>
-    </row>
-    <row r="38" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
+    <row r="39" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="16" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación subida fichero a cita
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E04D86C-59CE-4FC7-9397-508386EACBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A65EF6A-042F-4103-A469-E3307029B70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Como OCASIONAL, quiero loguearme</t>
   </si>
   <si>
-    <t>FLUTTER</t>
-  </si>
-  <si>
     <t>Como ADMIN, quiero crear un admin</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>HACER QUE PARA ELIMINAR O CANCELAR ALGO, HAYA QUE HACER UN ONLONGPRESSED, Y QUE EL ONTAP O EL ONPRESSED MUESTR EL SHOWSNACKBAR: showSnackbar("Deja pulsado para darte de baja", context);</t>
+  </si>
+  <si>
+    <t>PORQUE PETA SIEMPRE AL CARGAR EN PROD CON ESTE ERROR: Caused by: org.postgresql.util.PSQLException: ERROR: relation "mecanico" does not exist</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -405,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -740,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,14 +779,14 @@
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
@@ -791,11 +794,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -810,11 +813,11 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -829,11 +832,11 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -848,11 +851,11 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -867,11 +870,11 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -886,11 +889,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -905,18 +908,18 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="5" t="s">
@@ -924,11 +927,11 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -943,18 +946,18 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="6" t="s">
@@ -962,11 +965,11 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -981,11 +984,11 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -1000,11 +1003,11 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -1019,11 +1022,11 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1038,18 +1041,18 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="4" t="s">
@@ -1057,18 +1060,18 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="4" t="s">
@@ -1076,18 +1079,18 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="4" t="s">
@@ -1095,18 +1098,18 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="3" t="s">
@@ -1114,11 +1117,11 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -1133,11 +1136,11 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1152,18 +1155,18 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="5" t="s">
@@ -1171,11 +1174,11 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1"/>
     </row>
@@ -1190,18 +1193,18 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
@@ -1209,18 +1212,18 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="6" t="s">
@@ -1228,18 +1231,18 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="6" t="s">
@@ -1247,18 +1250,18 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="6" t="s">
@@ -1266,18 +1269,18 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="5" t="s">
@@ -1285,64 +1288,64 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="13" t="s">
-        <v>66</v>
+      <c r="F29" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="4" t="s">
-        <v>22</v>
+      <c r="F30" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>
@@ -1360,52 +1363,57 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="16" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="14" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación borra adjunto de una cita
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A65EF6A-042F-4103-A469-E3307029B70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB95BC7-CD5D-4B94-8908-751EC092E15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>PROGRESS</t>
   </si>
   <si>
     <t>PASAR A PROD APPLICATIONPROPERTIES</t>
@@ -365,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -395,9 +392,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -746,7 +740,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,8 +1319,8 @@
         <v>19</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="13" t="s">
-        <v>65</v>
+      <c r="F30" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
@@ -1377,43 +1371,43 @@
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
+    <row r="49" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="13" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
README, revisión y limpieza de código
</commit_message>
<xml_diff>
--- a/docs/documentacion/historias_usuario.xlsx
+++ b/docs/documentacion/historias_usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruiz.lomar22\Desktop\talleres-ruiz\docs\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\talleres-ruiz\docs\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE72459F-4F30-4BB0-8172-27853CBAF176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C15C314-8ADE-41A0-A486-F72333544B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Como ADMIN, quiero eliminar un mecánico o un admin</t>
   </si>
   <si>
-    <t>Como HABITUAL-ADMIN-MEC, quiero ver los detalles de una cita</t>
-  </si>
-  <si>
     <t>/auth/cita/</t>
   </si>
   <si>
@@ -150,15 +147,6 @@
     <t>Como ADMIN, MEC, HABITUAL, quiero modificar mi contraseña</t>
   </si>
   <si>
-    <t>ADMIN: mrl26 / admin1234</t>
-  </si>
-  <si>
-    <t>MEC: asp14 / mec1234</t>
-  </si>
-  <si>
-    <t>CLIENTE: jjml4 / cli1234</t>
-  </si>
-  <si>
     <t>/auth/cliente/me/citas</t>
   </si>
   <si>
@@ -216,28 +204,25 @@
     <t>Como ADMIN-MEC-HABITUAL, quiero hacer logout</t>
   </si>
   <si>
-    <t>Como ADMIN-MEC quiero ver mis detalles de un mecánico o admin</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>PASAR A PROD APPLICATIONPROPERTIES</t>
-  </si>
-  <si>
-    <t>SI SE ELIMINA UNA CITA EN TRÁMITE O ACEPTADA SE BORRAN LOS ADJUNTOS, Y SI HAY FOTOS, LAS QUE ESTÉN EN LA CARPETA???</t>
-  </si>
-  <si>
-    <t>README + SWAGGER + COLECCIÓN POSTMAN</t>
-  </si>
-  <si>
-    <t>BORRAR TODO PARA VER QUE NO PETA</t>
-  </si>
-  <si>
-    <t>BUSCAR FOTO QUE NO EXISTE PARA TRATAR EL ERROR</t>
-  </si>
-  <si>
-    <t>SI HAGO POST DE FICHERO SIN METER NADA, DA ERROR 500, PUEDE SER PORQUE LLAMO A FILESTORAGESYSTEM Y NO A STORAGE SERVICE. MIRAR EJEMPLO LUISMI</t>
+    <t>/auth/cita/mecanico/me</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC-HABITUAL, quiero ver los detalles de una cita</t>
+  </si>
+  <si>
+    <t>Como ADMIN-MEC quiero ver mis detalles de mecánico o admin</t>
+  </si>
+  <si>
+    <t>ADMIN: admin / admin</t>
+  </si>
+  <si>
+    <t>MEC: mec / mec</t>
+  </si>
+  <si>
+    <t>CLIENTE: cliente / cliente</t>
   </si>
 </sst>
 </file>
@@ -282,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,18 +316,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -388,15 +361,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,7 +706,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B43" sqref="B36:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +746,7 @@
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
@@ -783,7 +754,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="9" t="s">
@@ -802,7 +773,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="9" t="s">
@@ -821,11 +792,11 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -840,11 +811,11 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -859,11 +830,11 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -878,11 +849,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -897,18 +868,18 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="5" t="s">
@@ -916,7 +887,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="10" t="s">
@@ -935,18 +906,18 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="6" t="s">
@@ -954,11 +925,11 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -973,7 +944,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="9" t="s">
@@ -992,7 +963,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">
@@ -1011,11 +982,11 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1030,7 +1001,7 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="s">
@@ -1041,7 +1012,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="4" t="s">
@@ -1049,7 +1020,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="9" t="s">
@@ -1060,7 +1031,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="4" t="s">
@@ -1068,18 +1039,18 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="4" t="s">
@@ -1087,11 +1058,11 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1106,7 +1077,7 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="s">
@@ -1125,7 +1096,7 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9" t="s">
@@ -1144,18 +1115,18 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="5" t="s">
@@ -1163,7 +1134,7 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9" t="s">
@@ -1182,18 +1153,18 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
@@ -1201,11 +1172,11 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1220,7 +1191,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="9" t="s">
@@ -1231,7 +1202,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="6" t="s">
@@ -1239,7 +1210,7 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="9" t="s">
@@ -1250,7 +1221,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="6" t="s">
@@ -1258,18 +1229,18 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="3" t="s">
@@ -1277,18 +1248,18 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="3" t="s">
@@ -1296,18 +1267,18 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="6" t="s">
@@ -1315,26 +1286,26 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>
@@ -1350,54 +1321,41 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="17"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="14"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="15"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="14"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>